<commit_message>
Expand Summary sheet table
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1184C5E2-1965-3E42-9F96-77F7791BCBEC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BF79A8-9A09-844E-A260-52E22E4887A8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
@@ -155,15 +155,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -223,6 +214,15 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -339,18 +339,18 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:T6" totalsRowCount="1">
-  <autoFilter ref="Q1:T5" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:T9" totalsRowCount="1">
+  <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{586E8DC7-D719-8441-B4D4-56DD4B5ED5FC}" name="Sheets" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" dataDxfId="2">
-      <calculatedColumnFormula>COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]])</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="8">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" dataDxfId="1">
-      <calculatedColumnFormula>COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]])</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="7">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="count" dataDxfId="0">
-      <calculatedColumnFormula>COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]])</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="6">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -725,7 +725,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -784,7 +784,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -843,7 +843,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -902,7 +902,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -961,7 +961,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1020,7 +1020,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1033,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
-  <dimension ref="Q1:T6"/>
+  <dimension ref="Q1:T9"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,68 +1056,118 @@
       </c>
     </row>
     <row r="2" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R2" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S2" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T2" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]])</f>
-        <v>#REF!</v>
+      <c r="R2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="T2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
       </c>
     </row>
     <row r="3" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R3" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S3" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T3" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]])</f>
-        <v>#REF!</v>
+      <c r="R3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="T3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
       </c>
     </row>
     <row r="4" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R4" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S4" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T4" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]])</f>
-        <v>#REF!</v>
+      <c r="R4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="T4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R5" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S5" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T5" t="e">
-        <f ca="1">COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]])</f>
-        <v>#REF!</v>
+      <c r="R5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="T5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="Q6" t="s">
+      <c r="R6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="T6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="T7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="T8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q9" t="s">
         <v>13</v>
       </c>
-      <c r="T6">
-        <f ca="1">SUBTOTAL(103,Table2[cat3])</f>
-        <v>4</v>
+      <c r="R9">
+        <f ca="1">SUBTOTAL(109,Table2[cat1])</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f ca="1">SUBTOTAL(109,Table2[cat2])</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f ca="1">SUBTOTAL(109,Table2[cat3])</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix formulas in summary sheet table
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BF79A8-9A09-844E-A260-52E22E4887A8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F27A5E-1E76-974F-9D46-0BC27E1954B5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="7" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -155,6 +155,12 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -217,12 +223,6 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -346,11 +346,11 @@
     <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="7">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="1">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="6">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -681,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -725,7 +725,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -784,7 +784,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -843,7 +843,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -902,7 +902,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -961,7 +961,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1020,7 +1020,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
   <dimension ref="Q1:T9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,11 +1061,11 @@
         <v/>
       </c>
       <c r="S2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
@@ -1075,11 +1075,11 @@
         <v/>
       </c>
       <c r="S3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
@@ -1089,11 +1089,11 @@
         <v/>
       </c>
       <c r="S4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
@@ -1103,11 +1103,11 @@
         <v/>
       </c>
       <c r="S5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
@@ -1117,11 +1117,11 @@
         <v/>
       </c>
       <c r="S6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
@@ -1131,11 +1131,11 @@
         <v/>
       </c>
       <c r="S7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
@@ -1145,11 +1145,11 @@
         <v/>
       </c>
       <c r="S8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Add category column to template
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F27A5E-1E76-974F-9D46-0BC27E1954B5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B37C42-6892-CD46-8251-41D83E01714F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="7" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
   <si>
     <t>Beautiful header!</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Some text</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -155,12 +158,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -223,6 +220,12 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -237,11 +240,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4F0E2C1-E48C-5647-AB86-88BA3821CD25}" name="Table1" displayName="Table1" ref="A3:H4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:H4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4F0E2C1-E48C-5647-AB86-88BA3821CD25}" name="Table1" displayName="Table1" ref="A3:I4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5D144077-5340-C544-9C9C-2FDB5C64D9C1}" name="name"/>
     <tableColumn id="2" xr3:uid="{2769D270-9B14-0943-BE3E-DE7D72687DED}" name="user_id"/>
+    <tableColumn id="10" xr3:uid="{0BE1084E-8627-B84D-968D-A84597E8CABA}" name="category"/>
     <tableColumn id="3" xr3:uid="{6CF4DBC8-B6E5-654E-A0CA-01DF8E331439}" name="A_text"/>
     <tableColumn id="4" xr3:uid="{A9996655-F641-5E44-BA0F-F0BFBA7AB45C}" name="A_1"/>
     <tableColumn id="5" xr3:uid="{FAFEC879-6C4D-6A48-8609-C7739219A95C}" name="B_1"/>
@@ -254,11 +258,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0E5D0480-9496-AB4B-8184-166C7D5FF4E4}" name="Table14" displayName="Table14" ref="A3:H4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:H4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0E5D0480-9496-AB4B-8184-166C7D5FF4E4}" name="Table14" displayName="Table14" ref="A3:I4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{667A8344-5AF2-9C42-8DFB-370D089DDB3B}" name="name"/>
     <tableColumn id="2" xr3:uid="{72CFD6A0-3D4D-0B4C-8060-A98C98FEE870}" name="user_id"/>
+    <tableColumn id="9" xr3:uid="{457A3F1F-352B-EF4C-BBF2-EEFB12ED5C44}" name="category"/>
     <tableColumn id="3" xr3:uid="{CAED5513-2AB4-1D4B-806E-8D2A8F8A8706}" name="A_text"/>
     <tableColumn id="4" xr3:uid="{07AC23A7-CCA5-3E41-98C1-1DF7BB44B513}" name="A_1"/>
     <tableColumn id="5" xr3:uid="{78410EE7-9F55-3349-B50C-6D86E2A19DDF}" name="B_1"/>
@@ -271,11 +276,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4B934371-BE2D-7F48-A1B2-F86ABE16A106}" name="Table145" displayName="Table145" ref="A3:H4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:H4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4B934371-BE2D-7F48-A1B2-F86ABE16A106}" name="Table145" displayName="Table145" ref="A3:I4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{858ED57A-15E6-AF40-9EC8-7A2B3B28650D}" name="name"/>
     <tableColumn id="2" xr3:uid="{5D40EA9E-19D2-494E-AE35-CD311FB2C67C}" name="user_id"/>
+    <tableColumn id="9" xr3:uid="{7967AE1D-371B-454D-9722-E0F9945FF8C8}" name="category"/>
     <tableColumn id="3" xr3:uid="{BA1151D2-EDBF-BE46-A2C1-0D86059D750F}" name="A_text"/>
     <tableColumn id="4" xr3:uid="{23FD9E9D-76CF-DF43-A6F5-2EA04FC78FB5}" name="A_1"/>
     <tableColumn id="5" xr3:uid="{132F12DF-F1C0-6442-AE11-F58D505FAC94}" name="B_1"/>
@@ -288,11 +294,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{17D49667-BAEF-9748-80A1-482AA8DAF479}" name="Table1456" displayName="Table1456" ref="A3:H4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:H4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{17D49667-BAEF-9748-80A1-482AA8DAF479}" name="Table1456" displayName="Table1456" ref="A3:I4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{1D6F2727-5F74-434C-BE13-64E1DB4A73EE}" name="name"/>
     <tableColumn id="2" xr3:uid="{9A363F56-382A-AC4A-80FD-D17B99B63649}" name="user_id"/>
+    <tableColumn id="9" xr3:uid="{772BEACA-F039-524F-ACB3-AD60E80F5103}" name="category"/>
     <tableColumn id="3" xr3:uid="{AF42329A-3188-784A-BD2F-2E3DBD0CCA46}" name="A_text"/>
     <tableColumn id="4" xr3:uid="{CF9888AB-99A7-3C4F-8C3A-BE8AC62F31F1}" name="A_1"/>
     <tableColumn id="5" xr3:uid="{9E4D89F1-DAF0-4041-A676-2F514FBB2895}" name="B_1"/>
@@ -305,11 +312,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E80216C2-6049-0E45-A488-7935052DCC7D}" name="Table14567" displayName="Table14567" ref="A3:H4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:H4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E80216C2-6049-0E45-A488-7935052DCC7D}" name="Table14567" displayName="Table14567" ref="A3:I4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{CF0E1888-4D1D-4B48-AF28-1A6C183E9434}" name="name"/>
     <tableColumn id="2" xr3:uid="{42ADE484-0FE0-3445-A0A8-54A2ECA26974}" name="user_id"/>
+    <tableColumn id="9" xr3:uid="{0F9A9C28-EE1F-0C4D-8250-1257C754EF4B}" name="category"/>
     <tableColumn id="3" xr3:uid="{A38AD2D2-A461-8C49-9CF6-9F499D03F936}" name="A_text"/>
     <tableColumn id="4" xr3:uid="{1BFE15E9-30DE-5349-ABD5-A9990FB739B0}" name="A_1"/>
     <tableColumn id="5" xr3:uid="{33AB9F02-1401-0F42-BB3E-E962C931C725}" name="B_1"/>
@@ -322,11 +330,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C6489835-394E-4446-A2D5-0FA82B2FF1C4}" name="Table145678" displayName="Table145678" ref="A3:H4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:H4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C6489835-394E-4446-A2D5-0FA82B2FF1C4}" name="Table145678" displayName="Table145678" ref="A3:I4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0A5F64D9-06BB-6145-A70E-9516F166FB0B}" name="name"/>
     <tableColumn id="2" xr3:uid="{D17661E2-78BE-3947-92B3-7B1267DD7B7F}" name="user_id"/>
+    <tableColumn id="9" xr3:uid="{BCBADC4A-9904-D449-8997-32244F115DC7}" name="category"/>
     <tableColumn id="3" xr3:uid="{E221B0EC-DD75-6948-A82C-68BA44F70550}" name="A_text"/>
     <tableColumn id="4" xr3:uid="{C27A457E-AFC1-1341-AFD9-F0DE465D1958}" name="A_1"/>
     <tableColumn id="5" xr3:uid="{C8C6D0DA-9F68-AE44-82A9-48EADD49665E}" name="B_1"/>
@@ -346,10 +355,10 @@
     <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="6">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -679,25 +688,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -705,144 +714,29 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A311409D-6B38-6242-ABE9-B305E97B0CA4}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762062D-DDBA-4F4E-9268-852CE2715EFE}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
@@ -854,27 +748,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4ED01C-8CF2-FB41-A181-1BF601A3A880}">
-  <dimension ref="A1:H3"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A311409D-6B38-6242-ABE9-B305E97B0CA4}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -882,26 +776,29 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
@@ -913,27 +810,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CEF2E4-EB8B-564D-B474-097143A90EED}">
-  <dimension ref="A1:H3"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762062D-DDBA-4F4E-9268-852CE2715EFE}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -941,26 +838,29 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
@@ -972,27 +872,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B8E05A-003B-5747-93F6-1BE3AC8386CD}">
-  <dimension ref="A1:H3"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4ED01C-8CF2-FB41-A181-1BF601A3A880}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1000,26 +900,29 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
@@ -1031,11 +934,135 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CEF2E4-EB8B-564D-B474-097143A90EED}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B8E05A-003B-5747-93F6-1BE3AC8386CD}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
   <dimension ref="Q1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix formula references to compound sheet names
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B37C42-6892-CD46-8251-41D83E01714F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F650D5-97FC-0544-AF71-C23798E4EE77}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="7" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -158,6 +158,15 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -217,15 +226,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -352,14 +352,14 @@
   <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{586E8DC7-D719-8441-B4D4-56DD4B5ED5FC}" name="Sheets" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="8">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="2">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="7">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="1">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="6">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -690,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -737,7 +737,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -799,7 +799,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -861,7 +861,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -923,7 +923,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -985,7 +985,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1047,7 +1047,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
   <dimension ref="Q1:T9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,99 +1084,99 @@
     </row>
     <row r="2" spans="17:20" x14ac:dyDescent="0.2">
       <c r="R2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
       </c>
       <c r="S2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="17:20" x14ac:dyDescent="0.2">
       <c r="R3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
       </c>
       <c r="S3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="17:20" x14ac:dyDescent="0.2">
       <c r="R4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
       </c>
       <c r="S4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="17:20" x14ac:dyDescent="0.2">
       <c r="R5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
       </c>
       <c r="S5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="17:20" x14ac:dyDescent="0.2">
       <c r="R6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
       </c>
       <c r="S6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="17:20" x14ac:dyDescent="0.2">
       <c r="R7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
       </c>
       <c r="S7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="17:20" x14ac:dyDescent="0.2">
       <c r="R8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
       </c>
       <c r="S8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
         <v/>
       </c>
       <c r="T8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT(Table2[[#This Row],[Sheets]]&amp;"!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Increase number of template sheets by 1
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F650D5-97FC-0544-AF71-C23798E4EE77}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E54384-EF59-A446-8E78-E355EB76C44B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="7" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
@@ -20,7 +20,8 @@
     <sheet name="WFA (4)" sheetId="6" r:id="rId5"/>
     <sheet name="WFA (5)" sheetId="7" r:id="rId6"/>
     <sheet name="WFA (6)" sheetId="8" r:id="rId7"/>
-    <sheet name="Player Summary" sheetId="2" r:id="rId8"/>
+    <sheet name="WFA (7)" sheetId="10" r:id="rId8"/>
+    <sheet name="Player Summary" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
   <si>
     <t>Beautiful header!</t>
   </si>
@@ -156,7 +157,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -348,17 +359,35 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{79780794-1A14-E149-BDE7-F0C9192CF018}" name="Table1456789" displayName="Table1456789" ref="A3:I4" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{5ECD203F-47B7-1C49-918C-391A2EF66395}" name="name"/>
+    <tableColumn id="2" xr3:uid="{5AF6A375-1267-CA40-9E7B-49F9148345E8}" name="user_id"/>
+    <tableColumn id="9" xr3:uid="{9D7C8ABA-4801-9649-B464-05055FA82205}" name="category"/>
+    <tableColumn id="3" xr3:uid="{3720B9F2-E63B-4E45-AE3A-3DC2E51D5CE1}" name="A_text"/>
+    <tableColumn id="4" xr3:uid="{F0837AA4-A074-E44F-8C06-BBEF37EB9632}" name="A_1"/>
+    <tableColumn id="5" xr3:uid="{CC688BF3-400B-1149-B4BF-548634E09872}" name="B_1"/>
+    <tableColumn id="6" xr3:uid="{39CFF6C8-8A9C-2840-B301-A7A453F9E334}" name="C_1"/>
+    <tableColumn id="7" xr3:uid="{7175A65A-ACE0-024E-91F9-2FE7C9AEB989}" name="D_1"/>
+    <tableColumn id="8" xr3:uid="{07050A69-0B47-5E48-826A-6AACD3D431B2}" name="Total Points"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:T9" totalsRowCount="1">
   <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{586E8DC7-D719-8441-B4D4-56DD4B5ED5FC}" name="Sheets" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="3">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -737,7 +766,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -799,7 +828,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -861,7 +890,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -923,7 +952,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -985,7 +1014,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1047,7 +1076,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1059,10 +1088,72 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261C7227-A39A-8E44-9429-16F902CF9086}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
   <dimension ref="Q1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Insert blank row above WFA dataframe
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13C697E-2896-A84F-ACB5-93F26149E6E7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F956642D-1BEA-5F4A-A4B4-572458675F6C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
@@ -705,15 +705,6 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -783,6 +774,15 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -807,8 +807,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4F0E2C1-E48C-5647-AB86-88BA3821CD25}" name="Table1" displayName="Table1" ref="A3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4F0E2C1-E48C-5647-AB86-88BA3821CD25}" name="Table1" displayName="Table1" ref="A4:I5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5D144077-5340-C544-9C9C-2FDB5C64D9C1}" name="name"/>
     <tableColumn id="2" xr3:uid="{2769D270-9B14-0943-BE3E-DE7D72687DED}" name="user_id"/>
@@ -825,8 +825,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0E5D0480-9496-AB4B-8184-166C7D5FF4E4}" name="Table14" displayName="Table14" ref="A3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0E5D0480-9496-AB4B-8184-166C7D5FF4E4}" name="Table14" displayName="Table14" ref="A4:I5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{667A8344-5AF2-9C42-8DFB-370D089DDB3B}" name="name"/>
     <tableColumn id="2" xr3:uid="{72CFD6A0-3D4D-0B4C-8060-A98C98FEE870}" name="user_id"/>
@@ -843,8 +843,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4B934371-BE2D-7F48-A1B2-F86ABE16A106}" name="Table145" displayName="Table145" ref="A3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4B934371-BE2D-7F48-A1B2-F86ABE16A106}" name="Table145" displayName="Table145" ref="A4:I5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{858ED57A-15E6-AF40-9EC8-7A2B3B28650D}" name="name"/>
     <tableColumn id="2" xr3:uid="{5D40EA9E-19D2-494E-AE35-CD311FB2C67C}" name="user_id"/>
@@ -861,8 +861,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{17D49667-BAEF-9748-80A1-482AA8DAF479}" name="Table1456" displayName="Table1456" ref="A3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{17D49667-BAEF-9748-80A1-482AA8DAF479}" name="Table1456" displayName="Table1456" ref="A4:I5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{1D6F2727-5F74-434C-BE13-64E1DB4A73EE}" name="name"/>
     <tableColumn id="2" xr3:uid="{9A363F56-382A-AC4A-80FD-D17B99B63649}" name="user_id"/>
@@ -879,8 +879,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E80216C2-6049-0E45-A488-7935052DCC7D}" name="Table14567" displayName="Table14567" ref="A3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E80216C2-6049-0E45-A488-7935052DCC7D}" name="Table14567" displayName="Table14567" ref="A4:I5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{CF0E1888-4D1D-4B48-AF28-1A6C183E9434}" name="name"/>
     <tableColumn id="2" xr3:uid="{42ADE484-0FE0-3445-A0A8-54A2ECA26974}" name="user_id"/>
@@ -897,8 +897,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C6489835-394E-4446-A2D5-0FA82B2FF1C4}" name="Table145678" displayName="Table145678" ref="A3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C6489835-394E-4446-A2D5-0FA82B2FF1C4}" name="Table145678" displayName="Table145678" ref="A4:I5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0A5F64D9-06BB-6145-A70E-9516F166FB0B}" name="name"/>
     <tableColumn id="2" xr3:uid="{D17661E2-78BE-3947-92B3-7B1267DD7B7F}" name="user_id"/>
@@ -915,8 +915,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{79780794-1A14-E149-BDE7-F0C9192CF018}" name="Table1456789" displayName="Table1456789" ref="A3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A3:I4" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{79780794-1A14-E149-BDE7-F0C9192CF018}" name="Table1456789" displayName="Table1456789" ref="A4:I5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5ECD203F-47B7-1C49-918C-391A2EF66395}" name="name"/>
     <tableColumn id="2" xr3:uid="{5AF6A375-1267-CA40-9E7B-49F9148345E8}" name="user_id"/>
@@ -937,13 +937,13 @@
   <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{586E8DC7-D719-8441-B4D4-56DD4B5ED5FC}" name="Sheets" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2194,11 +2194,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2212,47 +2210,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{940EFEA9-950F-D748-B85B-D3713E7607E3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{940EFEA9-950F-D748-B85B-D3713E7607E3}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2263,7 +2263,7 @@
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2273,11 +2273,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A311409D-6B38-6242-ABE9-B305E97B0CA4}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2291,43 +2289,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{A77AF65B-933F-7C41-90C5-86451E13AD84}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{A77AF65B-933F-7C41-90C5-86451E13AD84}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -2342,7 +2341,7 @@
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2352,11 +2351,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762062D-DDBA-4F4E-9268-852CE2715EFE}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2370,43 +2367,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{02D9FF4F-45DB-D149-BD4D-7F97445DD464}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{02D9FF4F-45DB-D149-BD4D-7F97445DD464}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -2421,7 +2419,7 @@
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2431,11 +2429,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4ED01C-8CF2-FB41-A181-1BF601A3A880}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2449,43 +2445,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{68A02ACB-FA85-AD4C-8E99-26A14AADF365}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{68A02ACB-FA85-AD4C-8E99-26A14AADF365}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -2500,7 +2497,7 @@
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2510,11 +2507,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CEF2E4-EB8B-564D-B474-097143A90EED}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2528,43 +2523,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{9B927F75-38C9-6E4B-A33A-DB9B19940C3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{9B927F75-38C9-6E4B-A33A-DB9B19940C3C}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -2579,7 +2575,7 @@
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2589,11 +2585,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B8E05A-003B-5747-93F6-1BE3AC8386CD}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2607,43 +2601,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{E63BE6ED-96F1-4B40-A75C-0041FD20BD79}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E63BE6ED-96F1-4B40-A75C-0041FD20BD79}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -2658,7 +2653,7 @@
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2668,11 +2663,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261C7227-A39A-8E44-9429-16F902CF9086}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2686,43 +2679,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{E54F7397-49F4-6243-B4ED-A69199BC87F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E54F7397-49F4-6243-B4ED-A69199BC87F0}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -2737,7 +2731,7 @@
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Write POC info from text file to README sheet
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F956642D-1BEA-5F4A-A4B4-572458675F6C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF84D94A-9F6B-FC4F-B7D1-3180E8917175}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="200">
   <si>
     <t>Beautiful header!</t>
   </si>
@@ -633,13 +633,16 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Points of Contact: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -658,6 +661,14 @@
     <font>
       <sz val="12"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -695,10 +706,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1248,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA852955-07A2-0848-B9B2-68EACE966615}">
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,17 +1273,17 @@
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1277,7 +1291,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1285,7 +1299,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1293,7 +1307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1301,47 +1315,53 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F9" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2185,7 +2205,11 @@
   <sortState ref="A5:A202">
     <sortCondition ref="A202"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="F9:G10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2196,7 +2220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
Add timing; correct app call; practice on one org; edit templateˆ
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF84D94A-9F6B-FC4F-B7D1-3180E8917175}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486E8105-F6AC-A241-A550-CBE1B5690187}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
     <sheet name="WFA" sheetId="1" r:id="rId2"/>
-    <sheet name="WFA (2)" sheetId="4" r:id="rId3"/>
-    <sheet name="WFA (3)" sheetId="5" r:id="rId4"/>
-    <sheet name="WFA (4)" sheetId="6" r:id="rId5"/>
-    <sheet name="WFA (5)" sheetId="7" r:id="rId6"/>
-    <sheet name="WFA (6)" sheetId="8" r:id="rId7"/>
-    <sheet name="WFA (7)" sheetId="10" r:id="rId8"/>
-    <sheet name="Player Summary" sheetId="2" r:id="rId9"/>
+    <sheet name="WFA (2)" sheetId="11" r:id="rId3"/>
+    <sheet name="WFA (3)" sheetId="12" r:id="rId4"/>
+    <sheet name="WFA (4)" sheetId="13" r:id="rId5"/>
+    <sheet name="WFA (5)" sheetId="14" r:id="rId6"/>
+    <sheet name="WFA (6)" sheetId="15" r:id="rId7"/>
+    <sheet name="WFA (7)" sheetId="16" r:id="rId8"/>
+    <sheet name="WFA (8)" sheetId="17" r:id="rId9"/>
+    <sheet name="Player Summary" sheetId="2" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="categories">README!$C$5:$C$7</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="228">
   <si>
     <t>Beautiful header!</t>
   </si>
@@ -44,27 +45,6 @@
     <t>Lighter sub-header</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>A_text</t>
-  </si>
-  <si>
-    <t>A_1</t>
-  </si>
-  <si>
-    <t>B_1</t>
-  </si>
-  <si>
-    <t>C_1</t>
-  </si>
-  <si>
-    <t>D_1</t>
-  </si>
-  <si>
     <t>Sheets</t>
   </si>
   <si>
@@ -80,9 +60,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Total Points</t>
-  </si>
-  <si>
     <t>README!</t>
   </si>
   <si>
@@ -636,6 +613,114 @@
   </si>
   <si>
     <t xml:space="preserve">Points of Contact: </t>
+  </si>
+  <si>
+    <t>player_id</t>
+  </si>
+  <si>
+    <t>player_name</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>country_01</t>
+  </si>
+  <si>
+    <t>description_01</t>
+  </si>
+  <si>
+    <t>amount_01</t>
+  </si>
+  <si>
+    <t>country_02</t>
+  </si>
+  <si>
+    <t>description_02</t>
+  </si>
+  <si>
+    <t>amount_02</t>
+  </si>
+  <si>
+    <t>country_03</t>
+  </si>
+  <si>
+    <t>description_03</t>
+  </si>
+  <si>
+    <t>amount_03</t>
+  </si>
+  <si>
+    <t>country_04</t>
+  </si>
+  <si>
+    <t>description_04</t>
+  </si>
+  <si>
+    <t>amount_04</t>
+  </si>
+  <si>
+    <t>country_05</t>
+  </si>
+  <si>
+    <t>description_05</t>
+  </si>
+  <si>
+    <t>amount_05</t>
+  </si>
+  <si>
+    <t>country_06</t>
+  </si>
+  <si>
+    <t>description_06</t>
+  </si>
+  <si>
+    <t>amount_06</t>
+  </si>
+  <si>
+    <t>country_07</t>
+  </si>
+  <si>
+    <t>description_07</t>
+  </si>
+  <si>
+    <t>amount_07</t>
+  </si>
+  <si>
+    <t>country_08</t>
+  </si>
+  <si>
+    <t>description_08</t>
+  </si>
+  <si>
+    <t>amount_08</t>
+  </si>
+  <si>
+    <t>country_09</t>
+  </si>
+  <si>
+    <t>description_09</t>
+  </si>
+  <si>
+    <t>amount_09</t>
+  </si>
+  <si>
+    <t>country_10</t>
+  </si>
+  <si>
+    <t>description_10</t>
+  </si>
+  <si>
+    <t>amount_10</t>
+  </si>
+  <si>
+    <t>total_amount</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>sheet</t>
   </si>
 </sst>
 </file>
@@ -717,7 +802,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -797,6 +882,16 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -820,133 +915,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4F0E2C1-E48C-5647-AB86-88BA3821CD25}" name="Table1" displayName="Table1" ref="A4:I5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5D144077-5340-C544-9C9C-2FDB5C64D9C1}" name="name"/>
-    <tableColumn id="2" xr3:uid="{2769D270-9B14-0943-BE3E-DE7D72687DED}" name="user_id"/>
-    <tableColumn id="10" xr3:uid="{0BE1084E-8627-B84D-968D-A84597E8CABA}" name="category"/>
-    <tableColumn id="3" xr3:uid="{6CF4DBC8-B6E5-654E-A0CA-01DF8E331439}" name="A_text"/>
-    <tableColumn id="4" xr3:uid="{A9996655-F641-5E44-BA0F-F0BFBA7AB45C}" name="A_1"/>
-    <tableColumn id="5" xr3:uid="{FAFEC879-6C4D-6A48-8609-C7739219A95C}" name="B_1"/>
-    <tableColumn id="6" xr3:uid="{68650094-31E7-174A-AD37-EEB88A5F055E}" name="C_1"/>
-    <tableColumn id="7" xr3:uid="{7AE73DB8-2D4B-9F40-933B-8030CEB60533}" name="D_1"/>
-    <tableColumn id="8" xr3:uid="{5E033501-682B-1D4E-B34C-33F7CF1D1249}" name="Total Points"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0E5D0480-9496-AB4B-8184-166C7D5FF4E4}" name="Table14" displayName="Table14" ref="A4:I5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{667A8344-5AF2-9C42-8DFB-370D089DDB3B}" name="name"/>
-    <tableColumn id="2" xr3:uid="{72CFD6A0-3D4D-0B4C-8060-A98C98FEE870}" name="user_id"/>
-    <tableColumn id="9" xr3:uid="{457A3F1F-352B-EF4C-BBF2-EEFB12ED5C44}" name="category"/>
-    <tableColumn id="3" xr3:uid="{CAED5513-2AB4-1D4B-806E-8D2A8F8A8706}" name="A_text"/>
-    <tableColumn id="4" xr3:uid="{07AC23A7-CCA5-3E41-98C1-1DF7BB44B513}" name="A_1"/>
-    <tableColumn id="5" xr3:uid="{78410EE7-9F55-3349-B50C-6D86E2A19DDF}" name="B_1"/>
-    <tableColumn id="6" xr3:uid="{F9AB5994-9EB1-CC45-B2DB-0D9315F08953}" name="C_1"/>
-    <tableColumn id="7" xr3:uid="{EDFE5C4E-A8AD-524B-862F-82EE64187EFB}" name="D_1"/>
-    <tableColumn id="8" xr3:uid="{F1C8196E-FAB4-8E4D-89CF-58AF57A21453}" name="Total Points"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4B934371-BE2D-7F48-A1B2-F86ABE16A106}" name="Table145" displayName="Table145" ref="A4:I5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{858ED57A-15E6-AF40-9EC8-7A2B3B28650D}" name="name"/>
-    <tableColumn id="2" xr3:uid="{5D40EA9E-19D2-494E-AE35-CD311FB2C67C}" name="user_id"/>
-    <tableColumn id="9" xr3:uid="{7967AE1D-371B-454D-9722-E0F9945FF8C8}" name="category"/>
-    <tableColumn id="3" xr3:uid="{BA1151D2-EDBF-BE46-A2C1-0D86059D750F}" name="A_text"/>
-    <tableColumn id="4" xr3:uid="{23FD9E9D-76CF-DF43-A6F5-2EA04FC78FB5}" name="A_1"/>
-    <tableColumn id="5" xr3:uid="{132F12DF-F1C0-6442-AE11-F58D505FAC94}" name="B_1"/>
-    <tableColumn id="6" xr3:uid="{7597651F-6315-6B4B-A10B-E856FBF3909D}" name="C_1"/>
-    <tableColumn id="7" xr3:uid="{BF914050-0E66-AC44-99B9-436429986B60}" name="D_1"/>
-    <tableColumn id="8" xr3:uid="{02707062-F37B-8E49-A3E8-51A9D0DDE657}" name="Total Points"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{17D49667-BAEF-9748-80A1-482AA8DAF479}" name="Table1456" displayName="Table1456" ref="A4:I5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{1D6F2727-5F74-434C-BE13-64E1DB4A73EE}" name="name"/>
-    <tableColumn id="2" xr3:uid="{9A363F56-382A-AC4A-80FD-D17B99B63649}" name="user_id"/>
-    <tableColumn id="9" xr3:uid="{772BEACA-F039-524F-ACB3-AD60E80F5103}" name="category"/>
-    <tableColumn id="3" xr3:uid="{AF42329A-3188-784A-BD2F-2E3DBD0CCA46}" name="A_text"/>
-    <tableColumn id="4" xr3:uid="{CF9888AB-99A7-3C4F-8C3A-BE8AC62F31F1}" name="A_1"/>
-    <tableColumn id="5" xr3:uid="{9E4D89F1-DAF0-4041-A676-2F514FBB2895}" name="B_1"/>
-    <tableColumn id="6" xr3:uid="{B859A818-A6BD-A347-BB75-25BAEE55BC91}" name="C_1"/>
-    <tableColumn id="7" xr3:uid="{43796472-797C-694B-8DD7-1D454DB60827}" name="D_1"/>
-    <tableColumn id="8" xr3:uid="{68580D99-152E-344C-A519-3B640B06E850}" name="Total Points"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E80216C2-6049-0E45-A488-7935052DCC7D}" name="Table14567" displayName="Table14567" ref="A4:I5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{CF0E1888-4D1D-4B48-AF28-1A6C183E9434}" name="name"/>
-    <tableColumn id="2" xr3:uid="{42ADE484-0FE0-3445-A0A8-54A2ECA26974}" name="user_id"/>
-    <tableColumn id="9" xr3:uid="{0F9A9C28-EE1F-0C4D-8250-1257C754EF4B}" name="category"/>
-    <tableColumn id="3" xr3:uid="{A38AD2D2-A461-8C49-9CF6-9F499D03F936}" name="A_text"/>
-    <tableColumn id="4" xr3:uid="{1BFE15E9-30DE-5349-ABD5-A9990FB739B0}" name="A_1"/>
-    <tableColumn id="5" xr3:uid="{33AB9F02-1401-0F42-BB3E-E962C931C725}" name="B_1"/>
-    <tableColumn id="6" xr3:uid="{2D95E078-0E8C-2C4C-B997-4094D066FEC0}" name="C_1"/>
-    <tableColumn id="7" xr3:uid="{57501ADD-8CFA-8443-ACF8-46A59F7B962E}" name="D_1"/>
-    <tableColumn id="8" xr3:uid="{A8CC73D5-1448-A440-B8F8-C70EAD7C45C8}" name="Total Points"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C6489835-394E-4446-A2D5-0FA82B2FF1C4}" name="Table145678" displayName="Table145678" ref="A4:I5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0A5F64D9-06BB-6145-A70E-9516F166FB0B}" name="name"/>
-    <tableColumn id="2" xr3:uid="{D17661E2-78BE-3947-92B3-7B1267DD7B7F}" name="user_id"/>
-    <tableColumn id="9" xr3:uid="{BCBADC4A-9904-D449-8997-32244F115DC7}" name="category"/>
-    <tableColumn id="3" xr3:uid="{E221B0EC-DD75-6948-A82C-68BA44F70550}" name="A_text"/>
-    <tableColumn id="4" xr3:uid="{C27A457E-AFC1-1341-AFD9-F0DE465D1958}" name="A_1"/>
-    <tableColumn id="5" xr3:uid="{C8C6D0DA-9F68-AE44-82A9-48EADD49665E}" name="B_1"/>
-    <tableColumn id="6" xr3:uid="{99088610-1E34-F747-A2B6-4915680B68C3}" name="C_1"/>
-    <tableColumn id="7" xr3:uid="{3AFF355E-3785-2049-8B5C-7B05E752CF44}" name="D_1"/>
-    <tableColumn id="8" xr3:uid="{25CB9EA5-B830-EE4D-802C-E2AA42D15CFD}" name="Total Points"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{79780794-1A14-E149-BDE7-F0C9192CF018}" name="Table1456789" displayName="Table1456789" ref="A4:I5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:I5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5ECD203F-47B7-1C49-918C-391A2EF66395}" name="name"/>
-    <tableColumn id="2" xr3:uid="{5AF6A375-1267-CA40-9E7B-49F9148345E8}" name="user_id"/>
-    <tableColumn id="9" xr3:uid="{9D7C8ABA-4801-9649-B464-05055FA82205}" name="category"/>
-    <tableColumn id="3" xr3:uid="{3720B9F2-E63B-4E45-AE3A-3DC2E51D5CE1}" name="A_text"/>
-    <tableColumn id="4" xr3:uid="{F0837AA4-A074-E44F-8C06-BBEF37EB9632}" name="A_1"/>
-    <tableColumn id="5" xr3:uid="{CC688BF3-400B-1149-B4BF-548634E09872}" name="B_1"/>
-    <tableColumn id="6" xr3:uid="{39CFF6C8-8A9C-2840-B301-A7A453F9E334}" name="C_1"/>
-    <tableColumn id="7" xr3:uid="{7175A65A-ACE0-024E-91F9-2FE7C9AEB989}" name="D_1"/>
-    <tableColumn id="8" xr3:uid="{07050A69-0B47-5E48-826A-6AACD3D431B2}" name="Total Points"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:T9" totalsRowCount="1">
   <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
   <tableColumns count="4">
@@ -960,6 +929,374 @@
     <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4F0E2C1-E48C-5647-AB86-88BA3821CD25}" name="Table1" displayName="Table1" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{5D144077-5340-C544-9C9C-2FDB5C64D9C1}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{2769D270-9B14-0943-BE3E-DE7D72687DED}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{0BE1084E-8627-B84D-968D-A84597E8CABA}" name="category"/>
+    <tableColumn id="3" xr3:uid="{6CF4DBC8-B6E5-654E-A0CA-01DF8E331439}" name="org"/>
+    <tableColumn id="4" xr3:uid="{A9996655-F641-5E44-BA0F-F0BFBA7AB45C}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{FAFEC879-6C4D-6A48-8609-C7739219A95C}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{68650094-31E7-174A-AD37-EEB88A5F055E}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{7AE73DB8-2D4B-9F40-933B-8030CEB60533}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{5E033501-682B-1D4E-B34C-33F7CF1D1249}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{2FF1C114-5D0D-974E-8562-1D17AC30FACD}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{EC151170-E6E0-A941-B1DA-88199FA594A3}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{C9FE4AF3-0F05-814F-98A5-6BA8CE5EE3D6}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{8DCB405E-E328-9E4F-805A-51C71698A2B2}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{1471C197-6529-C84F-AC4C-94F41D1505C8}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{E64875F5-9B37-B245-8872-F2D9450619F7}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{2F21554C-1139-744B-A9A3-B410AC619BCF}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{766FA4BA-1E0A-B94D-B2EB-0882F8114219}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{7A207EFD-6F26-4D40-B7C1-763C4101B11E}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{C182745E-8C76-C242-BF25-12A99CE114DF}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{F5C1A059-D393-1843-8699-30F0E92E96F7}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{774D5924-00E3-0345-980F-D05B2995C592}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{E6ACAE43-4EA8-6E49-AE35-40A04814D447}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{0CE3EE33-F74A-1547-AB0B-1E3C60B1C5A2}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{EBDD1C95-CD93-AE4A-9F83-C85D63AE587F}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{4343A4D5-F788-594E-971A-4466F46C5851}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{CDC4F177-68AD-2741-87A2-1959A6546BC3}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{4CF74E57-E712-AF4C-A7F0-541C573D9672}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{39A6B9E5-03D3-284C-AB71-022505078AAE}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{0CBC17E2-94A8-7342-B1BC-FB11E4EAEA29}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{92C0C039-3310-474C-853F-0CB8B9CA630C}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{77883B92-6B21-7848-8B36-B3C0DE2B8D65}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{BFBC9FEE-0187-7C4D-A4EB-B00CC054409A}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{127BF0BF-D984-9D41-9FFF-B0C8AD0B5CD0}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{04690C5B-917B-CD42-B6D6-A0CA7C16D9BC}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{258367CF-5968-1E4B-898F-54A0A3172768}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{5E26A978-2681-8946-9151-0D75F232EA99}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{358D4D63-8C4A-D746-BE61-96C09F7D5971}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F4C92118-7093-5043-B640-BEA20FD759DF}" name="Table14" displayName="Table14" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{540E18CB-0B5C-9646-95CC-3B3684D42CBA}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{5A8483D8-264F-9F4F-AFF3-F088A85518ED}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{88EE82AC-D19E-1146-B72A-60C89D00143F}" name="category"/>
+    <tableColumn id="3" xr3:uid="{5D747677-4011-DD49-A189-F2BC20AFB69F}" name="org"/>
+    <tableColumn id="4" xr3:uid="{CBEDF1D0-62F8-4943-AE3A-8A8AEF9A32B8}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{B46C365C-C47F-1646-B4B4-E6C7D1D9CB79}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{BE30FCC3-C5E3-A84C-847A-213FD53C4923}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{508567A2-CCF3-B044-9D1D-1C3DE83EA938}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{D5F7AEF9-8BE5-1F45-9B50-2677592A32B7}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{E9A26A54-4C48-D74B-8654-132F012EAD6A}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{3EF5F2EC-7CD7-ED4A-BBF0-FA6CE1EEE6F2}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{5C318862-29D7-6848-B6C8-5C40EA03FA40}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{34AA9631-BE0A-2E49-BBA3-9C0D8303054B}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{493CB323-1923-B24A-A25E-53A578CFE19C}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{6F75B0D3-A6BD-CE43-9918-847A46D1F177}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{3A078558-8B3C-A244-8595-A47ECE089A3E}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{2E60A536-D860-2049-91EB-D45A521657BE}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{E3202306-6190-5848-89BE-733FA4877F5C}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{05ED7325-AC9A-194D-8E13-77EA4E1B022C}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{216D9FEB-5CB0-9946-9539-39B481566736}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{DA535E53-0A93-CA4D-97E3-26883F668296}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{D94FCB8F-73FC-AC44-98EC-D6DC1FBE006D}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{A375C83F-368D-684E-89AF-F06F12ED8377}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{54F38824-FD76-994B-BE94-F37EA3B4CFD3}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{D795B376-185B-F242-9C47-7440EFC4B58A}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{195000BA-7FED-224B-9DD4-660AB6EE3F81}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{C4A52A53-F15E-CF40-9493-DD0C7C8ABD43}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{1CB7BE98-0393-B242-99DC-EF4917904B35}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{192D103B-D0C8-9945-AD8D-DE1DC17541B0}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{71933777-34E0-4C4D-89D3-F5D2A375EF7F}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{1A1A35FC-F9CE-1C42-9501-5A65E28971C6}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{FC03A515-1CA2-D542-9B8E-EE36AAF4D0E6}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{38091342-056E-8C40-9A92-5B0357195FE3}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{6833850F-AAF7-1F49-B940-18605A636ACB}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{64C67DE6-F0D6-E843-97A7-EDC258541C91}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{E9BE27C9-0C71-B94F-89D8-8EEE71C39584}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{8B20D501-935C-5143-B0E1-629E8672250B}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4840193D-A365-D643-AED9-600E598715EF}" name="Table145" displayName="Table145" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{CED75071-278E-2148-B8C7-11206CE2747B}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{283205E1-2D32-E544-88A5-4ACA1A96FDE5}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{B24FD384-8A7F-DE4C-9366-0BFA2D61AB13}" name="category"/>
+    <tableColumn id="3" xr3:uid="{3AED6006-FABF-FF4B-AB8C-A701A18B0A76}" name="org"/>
+    <tableColumn id="4" xr3:uid="{51D5B30C-469D-7042-964D-C052D5484B30}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{962AF2A4-0A2E-E947-A4E5-EC9153D9B655}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{BC7B8364-D4F5-0A42-9D86-34B2930DAE7D}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{FE7B4F79-017B-B041-B917-7B4A6AFA343D}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{401FD665-AB19-8D41-97C4-5197C91994BD}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{1A14CCF2-E696-5747-B7E6-693781FE14D3}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{D4F6F29A-4E2F-0943-B733-21A448C60DB2}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{80295CE3-02F7-314F-9F54-F74703227DB0}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{320DE74D-723B-B74B-B36F-CB16A4E08A3C}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{AB563CA7-EA18-5E4C-89EF-BA602EE6751C}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{47313BDA-EF96-F349-AA1D-D56FE4DE7D95}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{FD839496-1272-0447-803D-3486C3313AC3}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{13972011-9DA4-264B-BFFA-1FB3B65FE580}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{2C0106F3-F374-1046-8C24-01290CD5C49E}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{9E972214-1900-464E-9867-1D4C085E86E0}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{E5E76CA5-F38B-A342-A39F-A8295AE7E612}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{E4D4E237-267F-4F45-8CC8-5026D52FE4B9}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{65E4AD4F-6F73-FD43-A983-F56BF98D699E}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{515D7DEF-50C8-4D43-8D57-4CF666AD7378}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{C54C35C3-904F-6143-BED7-3B04ADF023D0}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{9AA2D742-3ABA-A344-8DED-E00DB4F3CB21}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{B18A5B16-14A8-0049-BFED-8FC199CE45BD}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{F3C212F3-66DE-544D-8415-AFE83641A34D}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{9961498F-AC60-7449-B9C5-18791602208A}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{9D1F78F2-57E2-094E-ACB1-69F8B8C23F88}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{9F64528A-B56A-8345-9F1E-644E948FCD6C}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{21E3F35C-E252-3144-B155-857FC9C899DC}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{3150A04E-0DCA-3246-A260-2D61A71E7CA4}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{4EEF5C5F-7DE6-BC43-B232-CF5A572C55FD}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{8381E806-3658-604C-95B9-54DF276D4E75}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{76CC717D-936D-7649-9FB8-1D31FC4BBAAA}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{64A67AE8-2EEC-A546-A4DF-BFA7987C6323}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{DB573167-E66E-1B40-B4D2-0955FB915473}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D754AE42-AEB7-B24A-BF87-3C848D924F50}" name="Table1456" displayName="Table1456" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{CCE1D0A1-05EF-8044-86A3-B90C7E37C63A}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{F4A81287-93BD-9241-ABBF-6A3EC62A6E9E}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{B4F799A4-7968-8B44-BF36-8A7297BD1E70}" name="category"/>
+    <tableColumn id="3" xr3:uid="{1056A34C-C0CE-4447-860C-67D6F8D3E3ED}" name="org"/>
+    <tableColumn id="4" xr3:uid="{6F82DA5B-F305-BB43-87A1-F82743E0D7B2}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{8C918EDC-F604-A842-B9B1-524CA82DB5F9}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{3EA4CA46-5FF6-D54B-A0C7-848CF090655F}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{A91BC19F-8FA7-A947-BA74-DAC0E8A2A1B3}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{09F3B98C-EC4E-DD47-A14B-62FEF78C3F31}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{B9EC4F72-8915-504C-B0B4-62435D9BB90C}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{2560CB02-5DAA-0D43-B410-16EC3EA93D22}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{E71E0E47-0815-B640-AAC5-994D6F95ACC6}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{FF56EBDB-C5BC-D344-8DC0-3750D43C16EF}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{B319A627-B0A7-5E46-B0B9-30FF8393D7FA}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{DD3AACB0-A903-2B42-AAC4-6D0FDF567307}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{AFD3818D-0F0E-D747-B4B0-BDA9E2531D7B}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{27BA2499-3168-6242-8925-DED8FC7D3469}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{9D0BADB9-15C9-6F44-8C4E-3E7032FF4402}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{B9E419C3-8CB7-1D45-A159-0766BE90B680}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{C649B0DE-80BF-634C-90C6-4228C2BD1165}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{93FC1835-0E0F-3C4C-98A2-2AD9EF28DD06}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{A349370D-11EC-414E-AAEA-F18BD7F168FA}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{F05659F1-80FD-A442-BF3B-66C4E9221BB5}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{BD1646CB-3949-EE4C-89FF-E6493DEDC55E}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{DA306460-B10E-4845-8671-B250F54C0669}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{D34E060A-E214-434E-9A4C-110735D1BBC4}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{40F06BF7-2599-AA49-ADE1-103A123FAA3F}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{99AAC538-908D-1D45-82B6-FF8CEBD726D0}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{1353B0E3-E08C-1F45-8552-15A4FBEE021C}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{A561EF5C-E30D-C54B-B3F3-B4A026E941D2}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{6372477E-8AE8-AA4D-B1E2-1DDE1413AF43}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{5981D2F9-097B-7440-91DF-66A06A1709BC}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{F7D3CED8-E1FC-9944-86D7-8C5E19B38129}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{0F6A25BC-D2D3-DC47-A68C-F3BEAE8330EC}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{7426DC8D-B14F-E046-B69D-D0FECDB6CB17}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{125CFF16-00CC-A04E-8CE2-103EEE71B422}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{3ACF461A-2071-F747-AAE1-FC6FBB32227D}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{844727B7-9474-A54A-93BC-A781BEE929AA}" name="Table14567" displayName="Table14567" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{FC845C93-7786-5145-9491-DD0EDD72B1BA}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{E505A1E2-FFF8-3C4C-BCE9-3028A67F8B60}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{46B580D0-F698-6648-B71A-D4B886C04F2B}" name="category"/>
+    <tableColumn id="3" xr3:uid="{955DD3B8-66D1-2A44-9B7F-220EF8486EC7}" name="org"/>
+    <tableColumn id="4" xr3:uid="{64F09600-FB08-3D4C-84AF-702A51AB3BC4}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{E8AF604D-CBAC-0543-A5E1-E23164AB386C}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{63D42B69-5916-894C-A76B-777F69812A8C}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{DD4854F1-C94E-F44F-80C1-50D57856ABCE}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{EDB08771-524B-D449-A566-0BD2B725C33D}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{786A0237-5675-BE48-B9F0-204A6E9B50D3}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{6E5521F7-74BF-FD49-B268-0BDDBED105D1}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{AAA35FAC-B431-6948-A4FD-3AA7B9902642}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{16EED02B-4707-BF49-B0EE-E919292D5734}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{410847C3-D4B6-D34B-B0FB-D5E93579FD74}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{60920D58-D191-E048-B367-B52932C09B1E}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{3F73C685-02A9-F142-B61B-DEF157FAF421}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{77319D63-E011-E242-9095-9F8418566569}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{86522018-D44F-174A-8EAA-21AC83672B56}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{9BCBB7F1-9943-904F-8DD7-DC8F3BEA9EAA}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{435B4552-0ADD-634B-816A-EFF54093F950}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{DE538FFD-AC59-6D46-B312-2F20B0895A78}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{822F4279-FA7B-0B4A-9F55-12312CB0A4EB}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{A3EDBF31-7C12-744A-A669-6FAD1AEE44D7}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{1C96D558-1E88-104A-B21F-8477D685DC30}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{915B582F-43E1-9640-8C8D-171331A0AADE}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{72DC207F-AA1B-5A47-B12E-3B82351F9AAD}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{63050DE4-725B-9845-A644-33E282472564}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{7D9B7E2C-F707-5843-A252-02C1672DA74E}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{B3382B2E-07D8-4F4A-B233-A16F2742F34B}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{7642E098-7F8D-7946-B9A2-A86F1E6D1F53}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{E77BD31F-55A5-5140-A9E3-6680702DE93E}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{8DA2C568-3CC8-3F47-9410-B734357729C8}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{F9A29B5D-FC4D-DF4A-8737-C078E279F3B9}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{6109337D-6B43-CE4B-8237-D818FA6F3A3D}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{6E2F82B8-2E80-2748-B303-C61B11368316}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{910C93CC-A346-8C4E-8257-EFD5BA9F5A5E}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{570E8F6C-40AA-AB47-9285-98E734EFD6F6}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C140C4F8-0E02-964E-84DF-3E7782327907}" name="Table145678" displayName="Table145678" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{3753C3FC-FECE-BB4A-A73B-2209FD3B49ED}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{D9D5880A-CB6B-8145-8D90-58DB00405BCE}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{766A0885-54CB-CB41-AD07-919A1EC1C8B0}" name="category"/>
+    <tableColumn id="3" xr3:uid="{97944EA4-9CC9-824B-84AC-A96633AF4385}" name="org"/>
+    <tableColumn id="4" xr3:uid="{83A5A449-B299-8F4B-9042-3ACCAC4A31E4}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{16E883D5-96B9-6F4F-A419-8C7D8CDDEBC0}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{99195EA5-3D83-DE44-B82C-C7157A036564}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{1DAEB232-8045-3B45-BBF4-D4B45379C40B}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{1D28A996-342B-5F4D-9B65-4A14181E74FA}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{35275A66-1607-CC4C-94B7-C7554B99980F}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{93F209F7-4CCF-4E48-B4C2-B9FC2163F8F7}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{0549E580-2918-5441-BCCD-652D01CA3BD9}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{CB763342-FC85-6C4C-AD6C-B410311FED55}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{5F2503F3-C190-A94C-9E30-08A9C3E43632}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{B674F2DA-BAA9-5940-9064-65FF2AF70526}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{7D5B93A6-690B-4C4E-8E62-3F0A466F0B66}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{82718349-5B36-EE4C-A427-C4474C71DCDB}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{506B890B-B5B5-3A4A-A727-077CBF8C5CBB}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{97B4F0EE-6428-B54E-A419-7E7F6A3CBA77}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{012A8278-A091-424D-A1D4-590672441864}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{8B1C6D46-01AC-2347-B7F5-E6928B99ECC4}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{7C4B306F-0392-CC46-B557-B1C96D16DA69}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{FAC1355D-8F4B-DE4B-906C-1CEB7CE43B1E}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{AAFE42D1-3E05-8C4A-A205-134FC064D451}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{511B66D7-6C1C-CA43-B0E8-52E1C803E2AA}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{D04CDE92-FEC7-BC49-95CB-F125399A776C}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{E224BE52-928B-6B41-9A76-B15FF1F9F9B2}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{ED980B4C-EC90-1B40-BBB9-58FBAF6DE691}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{E6A3F001-C365-DB4F-9F12-AF68CE55B755}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{6745FA49-E3DB-A24B-B7E5-61F527052CD2}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{40E4FD08-F8B9-6748-8173-E58BF4ADE98E}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{5D58C9BD-291F-5046-A0E7-590350F845CA}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{2C7F9E3B-BF4A-6740-8059-A7E813B2527D}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{FB93DC6B-B821-054A-B65A-7D14C078362A}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{3E18713F-A66E-0842-9D85-909100C37AB6}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{A02F8FB4-B693-174E-8BA1-3394863AE859}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{7628F845-73EC-864D-B824-DC38A677EFF5}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F44BE205-9E75-BE47-8522-2E32D863EE11}" name="Table1456789" displayName="Table1456789" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{41D78F91-831C-E54C-859F-7628B0434029}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{6F716FBB-5FB9-5341-A13E-1F93DC512EC3}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{5A3D9A63-9495-1D4E-8BA6-B6CAC67C83DD}" name="category"/>
+    <tableColumn id="3" xr3:uid="{18CC54C6-9A77-0541-BE82-1E856C83ABAF}" name="org"/>
+    <tableColumn id="4" xr3:uid="{A7CE1131-349C-5147-8E92-AABE5AB7AC65}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{F333AD0A-7773-C34F-97E4-C58C2B58644E}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{34772E91-5025-C744-93EC-E3A9C7D5B4A5}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{1C5F0BD2-4574-5041-9274-3E405613AB91}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{8F6A809F-E407-A144-8C48-A10DDB773340}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{8D24D86A-AFD3-184D-9484-8971F147C0CD}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{87105D21-0F05-8748-BCA0-936ECE716F3D}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{282771F5-01AB-0344-B709-C6B36211766C}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{798B468A-9B0B-4144-B28A-BDCFBA407AD3}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{3A936287-A9BB-674E-941C-92FD82648F2D}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{70BA3A96-F145-CD4E-BB90-9537D192B6D7}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{17DD0C12-EE9D-3A44-83C7-00D91EA76D44}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{B59D9CA9-7946-EE4B-A36D-7DB5D745346D}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{4339AAC7-2BA0-BC40-9F9C-E30387A61846}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{78F222B1-124D-1D4B-9C1C-62FDDE42A9A0}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{566B36BB-D333-E445-9066-16F4DEA5E275}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{BFEA9D22-CC62-7946-B5A9-6949A9DBF699}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{24E01E13-FD39-8F4B-8B0C-396D8BB9F577}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{2DD04892-9D2F-4C4C-AEA4-611F3C6CCDE3}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{69CFADFE-434F-BA4A-B415-7F6394AD49CC}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{C32EBE43-DF6C-D149-95F1-146B90B3F253}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{9DB157D0-EDC9-9D45-8872-97EC514B5121}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{E036C0F7-7A40-0140-B00A-0C2E423F2880}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{F24F9473-9B25-624E-AD5C-4BAD40881FEF}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{545E3343-D59C-4748-B184-45DCC61F619C}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{087B8E64-E80F-0A4F-9E47-A98997849CA7}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{0DFEC8E7-44A1-2B4D-8AC4-8BA64D6CD9C0}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{BA9CF852-65E6-A949-AA71-E8346785C0A1}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{FD6A8512-7C87-574A-9F73-9D18B71BEFA2}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{58E3EE8E-FF2E-EF43-AEC6-EFA6E09A9BEF}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{8685739A-4EDE-504B-9DED-AB5FADBCA787}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{86046D92-9008-B74E-84BF-DCD1836ACEF4}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{7CEF558C-FE36-DD46-A597-38BA15F38A07}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{20B33D00-CB80-2D41-B3AF-E50F00BFF460}" name="Table145678911" displayName="Table145678911" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{F77CAB20-55B1-CF47-B723-5D8580A470F1}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{580477D0-5429-6840-BCCB-2C1944182298}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{D04F97CF-3E9F-E149-A7A0-45308B7D51CC}" name="category"/>
+    <tableColumn id="3" xr3:uid="{82B6AD9F-D314-4849-BAB1-730538D5D5FF}" name="org"/>
+    <tableColumn id="4" xr3:uid="{698A365E-CB41-7849-9C3B-1AF5FEA6B8DF}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{82362D64-2327-644C-B81B-4CBFA8529AFB}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{767557D3-136E-E642-8983-BD786C7B3963}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{FFCC39D6-6DBC-2D40-A004-DF2710B31A55}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{D2561E43-3859-FD4F-9BAB-A2D86E701AA2}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{C05CC94C-D1B6-4F43-983B-201915E5D19E}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{1AA7166A-30A9-9043-8436-009974341780}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{EA6B89E2-7F89-814C-B3E7-8D677646258C}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{D1C0A63C-9507-3A4E-AB61-C665A35781E8}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{21DB5DB3-855D-9B4F-B903-D23F99AC610E}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{ACCCB04C-7798-A946-A2AA-2E149FE74F70}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{AFB6ECD2-0E90-D641-A14B-4DB2A4BA5264}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{A742A63A-D113-4444-B8CA-F205D6DE4C75}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{7BA3B6BB-E276-D64D-AA1F-109149416AB8}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{BABA3142-26CF-C54F-9F76-9044D725CF15}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{ED700518-A042-9149-B086-8A044B75B358}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{B3146B49-8B31-F64B-AC9C-0E682CCF62D9}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{57B903E0-A3A1-E046-B6FF-5166C8CFF6DB}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{D97B537B-0C1F-0A47-8CDD-3C94BF506EF7}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{DB694185-C23E-634F-8B25-DE19B3713695}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{55F8991D-150F-6E41-AA6C-374B062C84EF}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{175F21DB-81DB-C643-8E47-0563BD31F488}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{F41C161E-9F9F-4A47-91FF-7E48D73D8E61}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{4787567B-5337-2443-A195-0A3BA7486077}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{3BDBF116-5705-5843-978B-AC4C96EF304E}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{FF393715-33C8-2F4E-A6EE-35FB52B2077B}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{99BDF6AB-675F-B94C-9BCE-55107A8B5F6C}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{74DF795E-AEA1-3949-B62E-BB2A3AAB1993}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{A4690A78-D46F-7F40-94ED-87E17266D71F}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{2255B1E6-D905-A245-AAD7-269D49CAE86E}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{6390C539-8695-C84A-8CA3-F8A3D6E6191F}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{677CB649-503E-0542-B162-2761F8E64386}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{B943E3AE-BAA4-1B48-AD68-CA064EBCDFE9}" name="sheet"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1264,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA852955-07A2-0848-B9B2-68EACE966615}">
   <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -1275,930 +1612,930 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2216,57 +2553,290 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
-  <dimension ref="A1:I4"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
+  <dimension ref="Q1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <f ca="1">SUBTOTAL(109,Table2[cat1])</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f ca="1">SUBTOTAL(109,Table2[cat2])</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f ca="1">SUBTOTAL(109,Table2[cat3])</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2296,72 +2866,159 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A311409D-6B38-6242-ABE9-B305E97B0CA4}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C462A751-1031-0949-9285-42676992FFFA}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{A77AF65B-933F-7C41-90C5-86451E13AD84}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{952CA2F4-F5C5-744E-8DF3-15E0C8507286}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90EF5967-6793-BC4F-97AD-FF42D37EEE55}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{368716B4-8F56-FA4E-A044-DDF41477615C}">
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
@@ -2374,72 +3031,159 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762062D-DDBA-4F4E-9268-852CE2715EFE}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE07979-14F5-8948-9300-4E4E7B0A01D6}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{02D9FF4F-45DB-D149-BD4D-7F97445DD464}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{239BD8D2-D9B4-C444-AE0A-2B3A4E6713B2}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BABBFFAA-B32C-F543-A661-A269F5C4C81A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D6BDDFF2-6D6B-9442-9816-339FBDD69485}">
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
@@ -2452,72 +3196,159 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4ED01C-8CF2-FB41-A181-1BF601A3A880}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585C59-3E72-B743-B1E8-945DF29C7481}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{68A02ACB-FA85-AD4C-8E99-26A14AADF365}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E95DE60E-FDAE-2243-A727-F17B1F312D66}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5FEE7329-7DA3-4D4D-BE2F-90DDE4ED7E83}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FAF30B2C-8087-734B-805A-6433FCD5EB30}">
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
@@ -2530,72 +3361,159 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CEF2E4-EB8B-564D-B474-097143A90EED}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97D729D-08F3-D54B-87E8-A8AA7FEB034A}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{9B927F75-38C9-6E4B-A33A-DB9B19940C3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{086C894D-0C0D-3B45-90C1-30D3076C678D}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FABE8194-74EE-3242-BA98-4BDF254E2C58}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDD5CF39-BBAC-7746-A48E-BA986D67B48A}">
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
@@ -2608,72 +3526,159 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B8E05A-003B-5747-93F6-1BE3AC8386CD}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D08C85B-EA60-8E4C-A136-689EA31F0137}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E63BE6ED-96F1-4B40-A75C-0041FD20BD79}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{285DE5BB-B9E5-2E4D-9C57-E70537212349}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{380C7926-3F2D-4B42-A7B1-05A9BDD503D0}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACA40D7A-4285-CA43-9877-B7F701BC0207}">
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
@@ -2686,72 +3691,159 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261C7227-A39A-8E44-9429-16F902CF9086}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8314CDE7-A0FA-1D49-99AB-A9049A024B03}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E54F7397-49F4-6243-B4ED-A69199BC87F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{23A4B3CC-F84F-5A40-800A-9EB2FF838348}">
       <formula1>categories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{098D58F2-026A-CB4F-9506-F2B0F83A8CF6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E9D9B5BE-803B-F74A-A3FE-52B68E632F95}">
           <x14:formula1>
             <xm:f>README!$A$5:$A$183</xm:f>
           </x14:formula1>
@@ -2764,148 +3856,166 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
-  <dimension ref="Q1:T9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6FB7D4-C486-5E45-B59A-00AF0A667487}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="Q1" t="s">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="R8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="17:20" x14ac:dyDescent="0.2">
-      <c r="Q9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9">
-        <f ca="1">SUBTOTAL(109,Table2[cat1])</f>
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <f ca="1">SUBTOTAL(109,Table2[cat2])</f>
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <f ca="1">SUBTOTAL(109,Table2[cat3])</f>
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{57111A93-7B70-8D45-AC79-85685DA58033}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{10F064ED-D3A8-5845-B6CA-0EDFE27759C5}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Skip fhand, use outfile for copy2ˆ
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny Torkelson\Documents\hello-world\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360C63D5-E384-4F3D-9D3C-8B4A1E8F533D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDB8DBE-DE49-454C-9F31-1CEDC779BD23}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="465" windowWidth="26400" windowHeight="19035" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="8" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
     <sheet name="WFA" sheetId="1" r:id="rId2"/>
-    <sheet name="Player Summary" sheetId="2" r:id="rId3"/>
+    <sheet name="WFA (2)" sheetId="10" r:id="rId3"/>
+    <sheet name="WFA (3)" sheetId="11" r:id="rId4"/>
+    <sheet name="WFA (4)" sheetId="12" r:id="rId5"/>
+    <sheet name="WFA (5)" sheetId="13" r:id="rId6"/>
+    <sheet name="WFA (6)" sheetId="14" r:id="rId7"/>
+    <sheet name="WFA (7)" sheetId="15" r:id="rId8"/>
+    <sheet name="WFA (8)" sheetId="16" r:id="rId9"/>
+    <sheet name="Player Summary" sheetId="2" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="categories">README!$C$5:$C$7</definedName>
@@ -30,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="228">
   <si>
     <t>Beautiful header!</t>
   </si>
@@ -795,7 +802,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -833,6 +910,25 @@
   <autoFilter ref="A4:A183" xr:uid="{BABC2619-CC42-CF4B-BDE7-C088F189B67A}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{8E48F8E8-CE02-844F-B577-C05E0774DCCD}" name="countries"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:T9" totalsRowCount="1">
+  <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{586E8DC7-D719-8441-B4D4-56DD4B5ED5FC}" name="Sheets" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="9">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="8">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="7">
+      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,19 +981,322 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:T9" totalsRowCount="1">
-  <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{586E8DC7-D719-8441-B4D4-56DD4B5ED5FC}" name="Sheets" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="2">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="1">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="0">
-      <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BD2590D2-64D5-114A-9C54-D9EB05B97A2D}" name="Table14" displayName="Table14" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{9371C627-01D4-864E-A3B6-59FD3782AF8F}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{3C826EF6-507F-D643-A507-0A0F9F93D160}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{E47F4AA9-E84B-E04C-99CB-A731095D1B70}" name="category"/>
+    <tableColumn id="3" xr3:uid="{08AD3325-7FC1-514D-AD9A-6CBCF66B9772}" name="org"/>
+    <tableColumn id="4" xr3:uid="{A36DBDCD-6C02-1345-80B4-E08590E15AF7}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{396C7D14-9E18-AF42-930F-5DB62818FCDA}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{62915061-5107-4B48-9421-DE6A1DC491C5}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{4FDDDB4C-27E1-204E-87B7-8A56C7B53BEF}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{DFA3E11A-B813-4A4C-AD73-C34E276A33C8}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{05AB05A1-302E-B947-A79F-942958A5251A}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{0AA59AAC-2C5C-1548-81A7-206BD0085780}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{8CE848C0-CD73-674F-8FE4-F8252DC1195A}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{8E9A07DF-7065-484C-942C-7BBB58C0627A}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{F0255B19-5608-BA4E-AA36-374B10556062}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{3298F651-EDB5-8042-9C52-4FEA1C04283E}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{B2717D21-21A9-8B4A-8DD4-F26F972D8021}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{92D9B8E4-781D-9B4C-8DE6-EB5697E9A85B}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{998C8950-A2DA-2C49-BC7A-2BDA6D67CAF2}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{DEEC9031-4780-7C4E-94A0-EE79F820D26B}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{5C12FCE5-1FE9-5E4D-B05C-4D6637E4F65A}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{F35214A1-7F29-8442-82D6-FE26D73F04CC}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{74008A0B-F790-1942-B7D3-09666EE191D6}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{D349E61F-4313-B941-ADCD-33AB76F5FC4E}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{4493662B-9D9F-5746-8881-BD599A0ECC0A}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{58D97367-6767-5041-BA9F-B1AD00051D34}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{0692BAF5-0822-124E-9744-3709560D23DF}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{E60D5B68-1757-5D41-88C0-39DB27D38DFF}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{0F17A562-380D-D044-A163-2E61854EC7BC}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{0B80C91D-5D4E-8244-986F-51A89D45AF9F}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{A730A07B-DA4F-2A4B-BD29-F2DF8693DEAA}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{6ABEEEF9-99A5-E543-B062-6C646B3A3933}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{3CFCB66B-6437-CB42-B7D5-C884E2FC4802}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{ECA9EE0D-43AD-4742-8D63-E9684364E2BE}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{E616B857-F64E-F743-B145-A42006D11549}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{5956FB7B-54F3-1A44-BF89-FBBF498150E0}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{420EF1B3-F9D2-C549-9731-3A86B510EFBE}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{7DBACA9B-3B5B-3440-A84F-C4BAFAE32634}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3A4ACEDF-541F-4C43-9EA4-38D1136EE896}" name="Table145" displayName="Table145" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{8711BD38-9932-D84D-8473-9D73FB6FF4EF}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{4FED07DC-559E-B049-B720-BD66D85F654D}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{E97AB547-243E-694F-9C2C-16D08820C5FD}" name="category"/>
+    <tableColumn id="3" xr3:uid="{E4CCF4B4-1804-AA40-853F-E09868763EE2}" name="org"/>
+    <tableColumn id="4" xr3:uid="{FBBD2606-2FD2-2041-885A-88D6A3C577AB}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{482E29AD-ACAB-664A-A22B-0C07A0EC150C}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{B4DFBECA-C48C-2740-B347-C53645DAC8DA}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{BC766AAF-B08F-534F-AC74-3ED33AB9F143}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{4FE6564A-E5E2-D14E-9A70-86C501792E7E}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{B7581300-5CE1-A346-A14C-5F89FD86712F}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{6DDAAD4C-BE63-7B4C-A59F-BEE7C32F8016}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{60C80201-EE71-D04C-8C36-DABB10F75A1C}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{A85C6469-8FD0-EA44-B0D1-A22F4C8908BF}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{795A48C1-279A-4E48-B982-B774F12743B8}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{6AE867A6-B7AC-7643-8984-570A0E3D0531}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{4A9F9FC2-FC84-0941-8350-FA42B4B7CEE3}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{42AF86D7-2A31-9748-A11D-59B212F5BCB5}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{9045CF3F-A548-4943-BFB5-B15A3CBDB120}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{D36AFF98-336E-F54F-97D6-BAF7253CAEE4}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{C2EA0A6B-A687-AF47-9CDA-183FA2AEC7B6}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{82920B1B-9D2C-A64D-A918-958BDB90EFBB}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{9E31EC5C-850E-9340-8FFD-82BEC5C5494A}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{1DC5F8D4-1668-4B43-AB64-47A889D63DF3}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{66C78952-F9D6-D04E-9160-707C9E16F21B}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{173C10EE-3173-4846-BEFC-B41694B8423E}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{BF673F82-5900-B94B-A1D0-88D3A2CD62F6}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{F08E2893-448F-F04D-86D9-CC082127AC73}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{0FE299C6-E896-9443-9162-5FCB04EB355A}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{06CDABC2-E7F8-BA41-BF71-A85FA771B41F}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{DF407403-3F8B-8849-BD1C-2F6F6F4808A7}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{FDC3E462-D56A-0941-BCB1-775E8636FE90}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{A088F0CA-A830-8A45-B62B-FC8E406288CA}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{142AB0DC-D02D-B943-BA07-788B2808E5E6}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{831F64E0-F874-1449-AA8F-E16C2B7B51FA}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{93F27E9B-671A-194C-99B4-7B110D795DE5}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{4453310A-3E65-B54A-93D8-64AF0A48E137}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{8DAD5CD6-454A-104E-BF24-6C2BA92E502C}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7D9B5033-09B6-AD47-BDDF-2E8CDF185DDE}" name="Table1456" displayName="Table1456" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{0B2527E2-AE3E-F443-89B6-8D5B4E7D27DF}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{5F7EA5B5-7625-964B-B295-F162E847CEAB}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{F421FDFA-AFD7-7248-B0E0-C89037EA9DD6}" name="category"/>
+    <tableColumn id="3" xr3:uid="{CF309586-FA82-1E40-B93A-8D4DD846CF69}" name="org"/>
+    <tableColumn id="4" xr3:uid="{FF97AB53-1E2B-1948-8FA8-E72694744187}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{19EDD981-2A2D-6540-B747-F5D12E4A8137}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{454EF578-D2D7-CF42-87B2-B48880D01A3C}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{3B6D263A-DDEB-144E-8582-E38029E99D28}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{FA0DC702-D2C7-554D-8772-9E231FF5ECD4}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{079E19B7-FA59-A14D-B69D-14BFE459E6BF}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{1EC454DD-FDA6-3B41-9748-0FAA9AEA3483}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{EC57F5BC-9C37-0A45-8822-DFF0CE7A06AA}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{E43ECD85-B503-6C4E-9746-306FD4157120}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{A4BBCF99-73AB-3547-B204-77EB25C809AA}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{A43CDAEC-A3D5-7A4C-BB5E-8414554D4EA9}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{49F2336A-7210-D847-8768-33D1A20F36AE}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{7D2374C8-5F88-1243-83AE-B52C777047DD}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{ADE6D719-418F-EF4C-8D4B-67FB79CE5B68}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{A1037BB1-434A-A64A-A8BC-3301DA3B17D0}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{8ABE0295-EFC5-E24A-B1E2-671A221D26FC}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{2305B9D4-66E1-0948-B173-C727CE7A6118}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{426F0587-BB22-1549-8FDF-505FEAB67D5B}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{547AB0C6-942E-B24C-8CF1-7326ECEC5121}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{BE455671-3B6E-7E47-A627-959168DBD063}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{5AEFB80F-D6E8-764C-894B-C7DA23862A49}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{9D429C94-06A7-DE49-9122-63B55D3610D2}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{F3F40D93-172D-C440-B27F-B1C9D4B78144}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{5AE8F99F-813D-7C42-9311-C334A7D96CF5}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{E6B0BE5F-773C-A34A-B3CD-FE994E4A8199}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{71084F09-2BA4-0A47-A3CD-8ABD9E7976C5}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{790B3BF0-D70C-C54C-B71C-F4D329DF1B01}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{849EFDC2-F4AF-0E41-ABD2-7795377B754A}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{C005F42A-28FA-1146-AF07-7022C53C4CF6}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{E591F2C0-90F7-C24C-9452-01C72B37B2D2}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{C51D7C85-251A-924E-BC3A-E81A809C187F}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{12AB4A7D-0523-5E45-AE2F-0FC8270B1C89}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{2EC0C782-AA65-8048-9B5E-92F4D1F7DFB0}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4EC5A57F-AA31-6546-AC1E-3EE22681AE1B}" name="Table14567" displayName="Table14567" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{DCCEAC2A-8743-4D44-BB3F-944E54244295}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{F9A5D3F6-E231-A942-A491-0CF49B166CED}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{BCB116AE-100C-B145-9987-ED7878C3C3FB}" name="category"/>
+    <tableColumn id="3" xr3:uid="{F4F152E4-998A-1B43-B84F-3039CF003D60}" name="org"/>
+    <tableColumn id="4" xr3:uid="{174A080C-28F0-0B41-9830-E8CF9F3FEEA9}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{431C4A0D-8660-AF41-8438-CC95C83283BC}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{7D659FF6-4461-A542-B50A-BCB0253CC8A9}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{9826593D-7FC4-FC43-A360-F95F9AF63E0B}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{397493DA-76C1-F24E-A7F9-D0121D1A09CF}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{6DFEDB96-8C5E-6A40-9FD6-AB18D2416CB5}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{4F539C72-DD80-6A48-B5F5-8EB344BB46F0}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{C5949AFC-2A21-E74A-B66A-EBDBFC4F7E61}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{17FC988C-3216-2B41-ACA3-CD7F9AD78706}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{A0E50ADA-1211-8246-899A-516A70FF99B6}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{3CF8F010-D109-E94F-A4AD-36A0CAAAB51D}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{24BD5A8F-4B84-F743-AE71-F598E55BA0AE}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{210F771D-D78B-B147-A5F6-1FCDEDA7A43B}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{F0FE5A6A-B66D-8E4F-AB59-0761E7A4C2FF}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{466466A6-90EE-9E4C-B6D7-718BC46FB047}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{E4F5EBE0-9C74-D74F-9A92-3D519EE5D041}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{B44396ED-0F92-744F-9650-E141C3905908}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{1345D28B-A2EF-524E-B0AE-73B71C5FDC73}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{52531A1D-DB36-334E-A72C-011EC6088362}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{7379FACE-7A53-B54E-ACC3-F97C83D85B9E}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{DFD48F2C-DF18-F048-A2D7-665E8AC9B4D7}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{A37892FA-BC1F-DA4D-B0AA-519FA7A9E6FE}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{1B44C900-F24F-B646-BA49-72943D6C9F78}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{652764EC-AC07-5B40-8438-B663DA754416}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{CD19F960-8194-C349-AFA4-90AC1890F7C4}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{7950235B-3A50-8D46-B1B2-B8E1D109C908}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{DF0734F9-C7A5-D944-B6FF-37604FEC557D}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{B40A9948-D13D-164B-B696-4661F0E4CD64}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{3096E518-6024-244B-A09F-94678C4BA05B}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{F3094722-4A56-7442-9D97-93B58BCB5AE9}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{D8A6EBF8-EFB8-B345-96AF-3DC63C9BB77C}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{BFE4D9A9-CE6B-2847-8ACD-B1F8D79B1441}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{F7F535CE-B027-D54C-A6C7-946D85EB2E64}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E2AFD7C1-EE07-0745-891A-D96C2599454E}" name="Table145678" displayName="Table145678" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{2ACA359D-5319-0949-AB5D-3867505AFA01}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{6DC5BC11-16DD-CB41-A2E8-6897117E0358}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{F3A6E059-F475-1A42-B0E2-BAC8580A80FE}" name="category"/>
+    <tableColumn id="3" xr3:uid="{8F31B3AC-51CB-BE42-A85E-09ACEFFAE011}" name="org"/>
+    <tableColumn id="4" xr3:uid="{4DAB5A9A-6B8B-2745-A0C6-78155812AB1E}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{9F3EF05F-8695-654C-ADD3-58AEEC534C6D}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{B56CDAFC-C3DE-C444-8FE4-980219B155D9}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{E39744D7-92E4-B34A-BC2B-CA5A47BB4339}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{1CCC8013-3E3B-1A4E-BC9D-6992920119FD}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{53EA13D5-CDA8-1C4B-B7BF-84146DDB332E}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{00BA1D51-4FFA-664E-973A-D55D7FA08D9F}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{DF509DE6-A830-4C47-AD93-94CBD947E651}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{668649C1-323B-4547-ABFF-12D2C61EC365}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{4B69566E-9A14-1440-B2D5-6C7B2ACE09CB}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{C9A2C308-9E73-A144-B10C-279228A5B70E}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{76C62067-6024-DB40-9F70-5A755F4102AF}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{912C12D7-AC6C-6244-9720-9E5E9564FB6F}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{1FD1C6B3-EC46-1541-ADF0-48D03E1607BD}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{F322546D-4C90-D34E-9C6A-522BEBBEDB35}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{A3524A3C-215D-6A43-A171-4EE66B84E5ED}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{62BC0F95-BC5B-1A40-9D3F-0BCFD931FA27}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{1A0849D6-622C-1943-BF9B-CB5B8D9C0F25}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{4D5AFDD0-1550-504C-8D5E-5AADB7C88272}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{0F65E9FF-D57D-EB42-BB2B-B4222F743E69}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{9F6AD6F9-2CAE-D845-915B-54042638943A}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{8C4EB44B-AAC3-DE4E-AD08-65160DE9DADA}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{CE10DDF1-BF45-A34A-8DE7-201688075725}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{FCC47180-203E-7E47-8614-729D8608223C}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{5FF23F2C-4F92-A244-A82D-FD4EC10FDA66}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{1B3D0E6F-3989-9E4A-9355-E571F5584C6E}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{C6EDFBBC-013C-5740-A84C-ACC416784C4B}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{3401BC27-77BB-C94F-BCB2-3A6461EFA2BE}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{E7FED351-DC2F-0B4B-BC87-62FC26B7D179}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{5C074EE6-6F33-774B-A250-C0D123FA2B25}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{B83784A7-9138-DE41-BF56-C3629D50C9D2}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{D9686343-8321-4E46-B676-9BE3FCE164EA}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{DE70BE9D-4141-3042-A712-554AD5B75AF5}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{54AD605F-4B0F-0A4B-9DE9-F2AB5F18DFA2}" name="Table1456789" displayName="Table1456789" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{75328739-1125-BC4D-97C8-41A25B140779}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{582875CF-E89A-9E49-9A1C-235289E17E74}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{B7BDD630-2861-834D-97C9-38EF8F81D515}" name="category"/>
+    <tableColumn id="3" xr3:uid="{18430834-B021-3343-8CFC-0ACF57F96919}" name="org"/>
+    <tableColumn id="4" xr3:uid="{8331B9E4-3B7F-FF42-811E-E05F05B78DD3}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{26CE2CDD-3961-E74F-8074-3B96E733D846}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{2355981C-809D-E447-9CCD-58E01EA5CA14}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{C00EA941-706E-2F4A-9428-0BE05C58A463}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{9F278CFD-2C1E-8A49-BCF6-2A2D4A1CFABC}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{4362D587-5487-834A-886E-2B69ADD0EBEE}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{C6BB0745-933B-CA4B-BB31-EB1F858E92A2}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{4EEDFD6D-BC42-5C4A-A87F-164147569032}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{78F70DF4-99CE-0241-86F8-886634201953}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{AF4AAF51-9702-5344-BEB6-9B664FE9B1B4}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{B3404B84-47BE-7644-B5A9-B68A6A1AE65E}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{12641743-A7FB-1B4B-92F5-CF913206AE93}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{D6E154E7-8DD7-4944-8BDE-1A16B22C29D8}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{922BF97E-C8B2-C549-8E79-932849293110}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{60D6E091-1DFA-C04E-A30E-38E10953820A}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{14D794FB-034F-2D43-87F0-2FFB78B637EF}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{A4CD6E81-5357-B245-B7AC-0049510CAD52}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{2C2B88DF-F50D-0F4C-9219-CE9F47D04EB3}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{6859637A-F2F2-7C46-A5E2-0E0A30E32947}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{817164D4-2363-C241-88D3-6D9A4108BE02}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{361C4AB0-6E4F-DA41-86C3-4C1DB2D91935}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{E22B6600-558F-F84B-8ABB-52A480872E7F}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{F75C220A-DE14-C24C-A6C8-EFF04ADFFB6D}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{2F7B376B-C1A4-D142-A2DC-73D40A7F5F66}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{E5F554BE-3692-1245-9261-3CA317565849}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{A108D9CD-BB79-0645-9C92-3498A690DD37}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{2A499596-D0A2-634C-B44A-974D26277389}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{BD6083CF-2FF4-8D4F-A011-FD775D9FBA5C}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{47F47F1F-CBCD-6341-B366-6E5F72338596}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{CEF979C8-5FAA-E740-BEB2-41A639ADC0D8}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{D2CBF2C1-1B9A-1A41-952C-1D8E0782E8D8}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{8840A5A0-13A3-BE4F-BE48-CC4B9381680D}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{BD68FAD6-0696-E940-9517-D3C30DAACC5A}" name="sheet"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{66E04B64-5BDB-8948-A9E3-16AD778DA67C}" name="Table145678911" displayName="Table145678911" ref="A4:AK5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:AK5" xr:uid="{87379408-A040-4442-97A9-D2C0359F5E69}"/>
+  <tableColumns count="37">
+    <tableColumn id="1" xr3:uid="{FDD0772D-A8A8-3E46-AC70-3A24D5CC7A6F}" name="player_id"/>
+    <tableColumn id="2" xr3:uid="{FFF16B9F-12F1-954E-8357-67D993208CB2}" name="player_name"/>
+    <tableColumn id="10" xr3:uid="{1811DA3E-33CD-A24D-AA38-E90B8A26075F}" name="category"/>
+    <tableColumn id="3" xr3:uid="{5A8D385E-AF79-A543-A5EF-7821AD322785}" name="org"/>
+    <tableColumn id="4" xr3:uid="{0761CD42-B4E2-5447-981D-8BA52D828F47}" name="country_01"/>
+    <tableColumn id="5" xr3:uid="{A54BD31F-380C-6345-B8AA-6F10AF043330}" name="description_01"/>
+    <tableColumn id="6" xr3:uid="{A64B6B6D-9AEA-D54A-AD19-6992B102A512}" name="amount_01"/>
+    <tableColumn id="7" xr3:uid="{640F39A6-0ADF-4946-9149-C4F322AD370B}" name="country_02"/>
+    <tableColumn id="8" xr3:uid="{490F1F5F-877F-1E44-9B23-3A23F191502B}" name="description_02"/>
+    <tableColumn id="9" xr3:uid="{A5A153F1-DA6D-AE48-AB09-FA1841028DBD}" name="amount_02"/>
+    <tableColumn id="11" xr3:uid="{1C6E27E1-F7B4-E041-B76D-376274945759}" name="country_03"/>
+    <tableColumn id="12" xr3:uid="{5A29C6ED-3CCB-0243-8D4D-7A619504CDC7}" name="description_03"/>
+    <tableColumn id="13" xr3:uid="{B0AA0530-3E5A-0E41-B2AA-FC81F0006FEE}" name="amount_03"/>
+    <tableColumn id="14" xr3:uid="{62550807-ADC9-CE46-A35E-23EAC77D87C9}" name="country_04"/>
+    <tableColumn id="15" xr3:uid="{70675CD6-AD5A-6C40-B9F7-2A3DF9002D44}" name="description_04"/>
+    <tableColumn id="16" xr3:uid="{C561FC01-8111-2A48-A862-12695C58A073}" name="amount_04"/>
+    <tableColumn id="17" xr3:uid="{6FD3C91A-8EA9-C14A-9AAD-04AA5C152997}" name="country_05"/>
+    <tableColumn id="18" xr3:uid="{4E5BF3BA-AC00-2749-A970-3A8E4AF6CE45}" name="description_05"/>
+    <tableColumn id="19" xr3:uid="{F20EB754-6A92-5945-AA7E-F94E2D037E62}" name="amount_05"/>
+    <tableColumn id="20" xr3:uid="{C720F0BA-C51F-DC4F-A453-8E59E23F572E}" name="country_06"/>
+    <tableColumn id="21" xr3:uid="{F7A7A637-186F-7D47-8443-8103652EB338}" name="description_06"/>
+    <tableColumn id="22" xr3:uid="{6CAE53C5-C8FE-F741-A567-24BD6C2363CB}" name="amount_06"/>
+    <tableColumn id="23" xr3:uid="{F30A2571-DC7C-B24B-BE16-49F18E91B40B}" name="country_07"/>
+    <tableColumn id="24" xr3:uid="{D99174CA-034B-A64C-855B-E3D7072E5727}" name="description_07"/>
+    <tableColumn id="25" xr3:uid="{C6AE8E2B-4D6D-7544-B308-110156AB74F1}" name="amount_07"/>
+    <tableColumn id="26" xr3:uid="{C9CA2121-DF39-D04C-BB7A-CA252FB0D67E}" name="country_08"/>
+    <tableColumn id="27" xr3:uid="{33952674-316C-B844-AD98-756F2D8B14E1}" name="description_08"/>
+    <tableColumn id="28" xr3:uid="{547A7779-A390-8947-BF3C-A9856E62B3CD}" name="amount_08"/>
+    <tableColumn id="29" xr3:uid="{DF46DDE3-BB81-BF45-B401-0C1E1F098A20}" name="country_09"/>
+    <tableColumn id="30" xr3:uid="{C5D7F033-8BD6-CF4E-BB8C-33E94740C5E0}" name="description_09"/>
+    <tableColumn id="31" xr3:uid="{C167A9F5-428D-DC43-AAE3-A5A64196CD8E}" name="amount_09"/>
+    <tableColumn id="32" xr3:uid="{E15DA7D1-FB2B-EE4D-975D-DAA216970F29}" name="country_10"/>
+    <tableColumn id="33" xr3:uid="{C849C33C-8B6B-7C4F-A41B-DE65356E95F3}" name="description_10"/>
+    <tableColumn id="34" xr3:uid="{CEF10B2E-08D9-D74D-95ED-9F59182A56EB}" name="amount_10"/>
+    <tableColumn id="35" xr3:uid="{B0EC6D25-8542-8B4E-BD23-C5C3884F12D0}" name="total_amount"/>
+    <tableColumn id="36" xr3:uid="{B3C04788-C900-BE46-A527-F79523D3D598}" name="comments"/>
+    <tableColumn id="37" xr3:uid="{02D99031-1540-DC4B-B344-37169300EDBC}" name="sheet"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1206,22 +1605,22 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1229,7 +1628,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1237,7 +1636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1245,7 +1644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1253,12 +1652,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1267,874 +1666,874 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>189</v>
       </c>
@@ -2154,58 +2553,205 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
+  <dimension ref="Q1:T9"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T2" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T3" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T4" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T5" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T6" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T7" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="R8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
+        <v/>
+      </c>
+      <c r="S8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
+        <v/>
+      </c>
+      <c r="T8" t="str">
+        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <f ca="1">SUBTOTAL(109,Table2[cat1])</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f ca="1">SUBTOTAL(109,Table2[cat2])</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f ca="1">SUBTOTAL(109,Table2[cat3])</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -2320,7 +2866,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2350,148 +2896,1366 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
-  <dimension ref="Q1:T9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE2F54F-C369-8849-A475-F03233D1683E}">
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="R2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T2" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="R3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T3" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="R4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T4" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="R5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T5" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="R6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T6" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="R7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T7" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="R8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
-        <v/>
-      </c>
-      <c r="S8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</f>
-        <v/>
-      </c>
-      <c r="T8" t="str">
-        <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="17:20" x14ac:dyDescent="0.25">
-      <c r="Q9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9">
-        <f ca="1">SUBTOTAL(109,Table2[cat1])</f>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S9">
-        <f ca="1">SUBTOTAL(109,Table2[cat2])</f>
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <f ca="1">SUBTOTAL(109,Table2[cat3])</f>
-        <v>0</v>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{A1CF5050-376E-3B4D-82A2-F41E9BD6BDD0}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D14734F-1CB7-9B4A-97C7-FFC37F6CC6BC}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5 H5 K5 N5 Q5 T5 W5 Z5 AC5 AF5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72658281-6E09-EC4B-B661-0E3BEEE3F494}">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{3CA93760-756A-4643-B286-0D0ED12F40DE}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{52E94492-3154-7445-8456-35513CED0FF6}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5 H5 K5 N5 Q5 T5 W5 Z5 AC5 AF5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8967F94-87B3-034F-9855-ECA5959CF8A7}">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{1DBC40FB-18AE-4C44-A806-7798C3493F46}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A6768A0B-94B2-DD4A-B48F-92F2D50C86BE}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5 H5 K5 N5 Q5 T5 W5 Z5 AC5 AF5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CFA921-3E7A-EB47-92EC-9E7BB89F015D}">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{60FD49D6-698B-D749-BFF3-D654905D43A6}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{622FD860-503E-A04E-B6F7-B31A20B7436B}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5 H5 K5 N5 Q5 T5 W5 Z5 AC5 AF5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEE05C-99B6-CE40-91A3-C8E059D798F6}">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{5EC7E3A0-1B04-1544-90BC-3AA36C06F580}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F95292C3-5D45-1643-BDB7-73D80127DC66}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5 H5 K5 N5 Q5 T5 W5 Z5 AC5 AF5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0566687-5753-AB4E-B1F8-D68C88A51EE0}">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{6744D457-8F26-FA4B-8342-DA6E81E0C82E}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07A90F3C-93E3-A942-9963-3BD3A59BA2B9}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5 H5 K5 N5 Q5 T5 W5 Z5 AC5 AF5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34717C4-FEB1-E44A-A7F9-862481B65270}">
+  <dimension ref="A1:AK4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" t="s">
+        <v>199</v>
+      </c>
+      <c r="J4" t="s">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L4" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>207</v>
+      </c>
+      <c r="R4" t="s">
+        <v>208</v>
+      </c>
+      <c r="S4" t="s">
+        <v>209</v>
+      </c>
+      <c r="T4" t="s">
+        <v>210</v>
+      </c>
+      <c r="U4" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" t="s">
+        <v>213</v>
+      </c>
+      <c r="X4" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E4B4D988-21AB-3748-BB89-20DC18A79A5B}">
+      <formula1>categories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{067E6D02-9C1C-3142-A748-AE56D8394485}">
+          <x14:formula1>
+            <xm:f>README!$A$5:$A$183</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5 H5 K5 N5 Q5 T5 W5 Z5 AC5 AF5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add subtotals column to Player Summary
</commit_message>
<xml_diff>
--- a/my_template.xlsx
+++ b/my_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtork/Documents/hello-world/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny Torkelson\Documents\hello-world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDB8DBE-DE49-454C-9F31-1CEDC779BD23}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E25166-A8DA-4212-9917-04464652E3C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="26400" windowHeight="19040" activeTab="8" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
+    <workbookView xWindow="315" yWindow="465" windowWidth="26400" windowHeight="19035" activeTab="1" xr2:uid="{5D716E34-50E5-B840-B30A-21D3B41378B7}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="229">
   <si>
     <t>Beautiful header!</t>
   </si>
@@ -721,6 +721,9 @@
   </si>
   <si>
     <t>sheet</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
   </si>
 </sst>
 </file>
@@ -791,18 +794,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -874,15 +890,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -916,18 +923,21 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:T9" totalsRowCount="1">
-  <autoFilter ref="Q1:T8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{192BF46A-9649-8B4E-8896-803056231AD7}" name="Table2" displayName="Table2" ref="Q1:U9" totalsRowCount="1">
+  <autoFilter ref="Q1:U8" xr:uid="{6A9A0996-EFEF-DF4C-9E88-458BCE8CCC32}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{586E8DC7-D719-8441-B4D4-56DD4B5ED5FC}" name="Sheets" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{DE09EA39-C979-5A47-9805-55AF2104783F}" name="cat1" totalsRowFunction="sum" dataDxfId="3">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{EF51BCA5-4696-634C-BA66-86F8EE4A77E5}" name="cat2" totalsRowFunction="sum" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat2]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{0557DBE9-6871-AA48-A272-943B5D1D9153}" name="cat3" totalsRowFunction="sum" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C09584EE-299E-43E1-8FBA-7AFC926EB7E5}" name="Subtotal" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Table2[[#This Row],[cat1]:[cat3]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1605,22 +1615,22 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1628,7 +1638,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1636,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1644,7 +1654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1652,12 +1662,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1666,874 +1676,874 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>189</v>
       </c>
@@ -2555,15 +2565,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F05FE60-81FC-6243-933E-A4163DFA9B27}">
-  <dimension ref="Q1:T9"/>
+  <dimension ref="Q1:U9"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="17:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q1" t="s">
         <v>2</v>
       </c>
@@ -2576,8 +2586,11 @@
       <c r="T1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="17:21" x14ac:dyDescent="0.25">
       <c r="R2" t="str">
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
@@ -2590,8 +2603,12 @@
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U2" s="4">
+        <f ca="1">SUM(Table2[[#This Row],[cat1]:[cat3]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="17:21" x14ac:dyDescent="0.25">
       <c r="R3" t="str">
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
@@ -2604,8 +2621,12 @@
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U3" s="4">
+        <f ca="1">SUM(Table2[[#This Row],[cat1]:[cat3]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="17:21" x14ac:dyDescent="0.25">
       <c r="R4" t="str">
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
@@ -2618,8 +2639,12 @@
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U4" s="4">
+        <f ca="1">SUM(Table2[[#This Row],[cat1]:[cat3]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="17:21" x14ac:dyDescent="0.25">
       <c r="R5" t="str">
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
@@ -2632,8 +2657,12 @@
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U5" s="4">
+        <f ca="1">SUM(Table2[[#This Row],[cat1]:[cat3]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="17:21" x14ac:dyDescent="0.25">
       <c r="R6" t="str">
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
@@ -2646,8 +2675,12 @@
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U6" s="4">
+        <f ca="1">SUM(Table2[[#This Row],[cat1]:[cat3]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="17:21" x14ac:dyDescent="0.25">
       <c r="R7" t="str">
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
@@ -2660,8 +2693,12 @@
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U7" s="4">
+        <f ca="1">SUM(Table2[[#This Row],[cat1]:[cat3]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="17:21" x14ac:dyDescent="0.25">
       <c r="R8" t="str">
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat1]]),"")</f>
         <v/>
@@ -2674,8 +2711,12 @@
         <f ca="1">IFERROR(COUNTIF(INDIRECT("'"&amp;Table2[[#This Row],[Sheets]]&amp;"'!C:C"),Table2[[#Headers],[cat3]]),"")</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="U8" s="4">
+        <f ca="1">SUM(Table2[[#This Row],[cat1]:[cat3]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="17:21" x14ac:dyDescent="0.25">
       <c r="Q9" t="s">
         <v>6</v>
       </c>
@@ -2704,54 +2745,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99459FCD-1FF9-2B49-8070-93FF5C3CAE1C}">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -2866,7 +2907,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2903,50 +2944,50 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -3061,7 +3102,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3098,50 +3139,50 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -3256,7 +3297,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3293,50 +3334,50 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -3451,7 +3492,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3488,50 +3529,50 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -3646,7 +3687,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3683,50 +3724,50 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -3841,7 +3882,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3878,50 +3919,50 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -4036,7 +4077,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4069,54 +4110,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34717C4-FEB1-E44A-A7F9-862481B65270}">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -4231,7 +4272,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>